<commit_message>
Minor adjustments in Contact mapping
</commit_message>
<xml_diff>
--- a/Mappings/Contact - STU3.xlsx
+++ b/Mappings/Contact - STU3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="330" windowWidth="20835" windowHeight="9510"/>
+    <workbookView xWindow="240" yWindow="330" windowWidth="20835" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="outpatient" localSheetId="2">ContactTypeCodelijst!$H$5</definedName>
     <definedName name="virtual" localSheetId="2">ContactTypeCodelijst!$H$11</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -755,6 +755,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
@@ -785,7 +786,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1093,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1109,15 +1109,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1130,16 +1130,16 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="3"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="41"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="42"/>
       <c r="J2" s="4" t="s">
         <v>21</v>
       </c>
@@ -1150,10 +1150,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="42"/>
+      <c r="D3" s="43"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
         <v>8</v>
@@ -1175,10 +1175,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="43"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
         <v>10</v>
@@ -1368,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1492,13 +1492,13 @@
         <v>54</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>102</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F7" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38.25">
@@ -1509,13 +1509,13 @@
         <v>57</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>105</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1531,28 +1531,28 @@
     </row>
     <row r="10" spans="1:6">
       <c r="D10" s="33" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="E10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="D11" s="33" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="F11" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="38" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1580,15 +1580,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
       <c r="H2" s="30" t="s">
         <v>85</v>
       </c>

</xml_diff>